<commit_message>
hint system and formatting
</commit_message>
<xml_diff>
--- a/src/data/data.xlsx
+++ b/src/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\samsat-quiz-app\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF76EC80-5640-4A46-AB7F-B6E45478A4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109270B9-C61D-43A0-9727-33D4CF9B17C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -414,7 +414,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -463,10 +463,10 @@
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(1, 4)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <f ca="1">RANDBETWEEN(1, 4)</f>
+        <f ca="1">F2</f>
         <v>1</v>
       </c>
     </row>
@@ -488,11 +488,11 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:G13" ca="1" si="0">RANDBETWEEN(1, 4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G3">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f t="shared" ref="G3:G13" ca="1" si="1">F3</f>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -513,10 +513,10 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -538,10 +538,10 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -566,8 +566,8 @@
         <v>3</v>
       </c>
       <c r="G6">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -591,7 +591,7 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -613,11 +613,11 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -638,11 +638,11 @@
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -663,11 +663,11 @@
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -688,11 +688,11 @@
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G11">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -713,10 +713,10 @@
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G12">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -738,11 +738,11 @@
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
got bg images working for each question
</commit_message>
<xml_diff>
--- a/src/data/data.xlsx
+++ b/src/data/data.xlsx
@@ -5,16 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\samsat-quiz-app\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\quiz-app\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB861A16-0784-44B1-85BF-B48BCFABB488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF5CB26-0861-45F7-B5A7-EFB33ED86CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Debug Questions" sheetId="1" r:id="rId1"/>
-    <sheet name="Quiz 1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="20">
   <si>
     <t>Question</t>
   </si>
@@ -93,6 +92,9 @@
   </si>
   <si>
     <t>Absolutely?</t>
+  </si>
+  <si>
+    <t>Background</t>
   </si>
 </sst>
 </file>
@@ -410,19 +412,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I7" sqref="I7:N26"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,8 +447,11 @@
       <c r="G1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -470,7 +476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -495,7 +501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -513,14 +519,14 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -545,7 +551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -570,7 +576,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -588,14 +594,14 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -613,14 +619,14 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -638,14 +644,14 @@
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -663,14 +669,14 @@
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -695,7 +701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -713,14 +719,14 @@
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -743,45 +749,6 @@
       <c r="G13">
         <f t="shared" ca="1" si="1"/>
         <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60AC7D30-E8A3-417D-8B8C-CDA16C368AED}">
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tried to make background customization work
</commit_message>
<xml_diff>
--- a/src/data/data.xlsx
+++ b/src/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\quiz-app\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29603567-C570-429A-A037-8B0844FF1B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4A8A27-D52C-4CBC-A518-D296FA51F709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="67">
   <si>
     <t>Question</t>
   </si>
@@ -95,12 +95,6 @@
     <t>Absolutely?</t>
   </si>
   <si>
-    <t>HintImage</t>
-  </si>
-  <si>
-    <t>BackgroundImage</t>
-  </si>
-  <si>
     <t>In the 1500s, Leonardo da Vinci invented a cart that followed a set path.</t>
   </si>
   <si>
@@ -234,6 +228,15 @@
   </si>
   <si>
     <t>True or False?</t>
+  </si>
+  <si>
+    <t>https://cdn.pixabay.com/photo/2019/05/18/13/34/twigs-4211837__480.jpg</t>
+  </si>
+  <si>
+    <t>Background_Image</t>
+  </si>
+  <si>
+    <t>Hint_Image</t>
   </si>
 </sst>
 </file>
@@ -661,15 +664,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="64.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -695,10 +697,10 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="I1" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -719,11 +721,17 @@
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(1, COUNTA(B2:E2))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G2">
         <f t="shared" ref="G2:G13" ca="1" si="0">F2</f>
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -744,11 +752,11 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F14" ca="1" si="1">RANDBETWEEN(1, COUNTA(B3:E3))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -769,11 +777,11 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -794,11 +802,11 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -844,11 +852,11 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -869,11 +877,11 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -894,11 +902,11 @@
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -919,11 +927,11 @@
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -944,11 +952,11 @@
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -969,11 +977,11 @@
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1003,7 +1011,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B14" s="11" t="b">
         <v>1</v>
@@ -1070,186 +1078,186 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="F2" s="1">
         <v>3</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="F3" s="1">
         <v>3</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="F4" s="1">
         <v>4</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="F5" s="1">
         <v>1</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="E7" s="9" t="s">
         <v>49</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="F7" s="1">
         <v>3</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B8" s="9" t="b">
         <v>1</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>54</v>
-      </c>
       <c r="F8" s="1">
         <v>1</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added background image customization
</commit_message>
<xml_diff>
--- a/src/data/data.xlsx
+++ b/src/data/data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\quiz-app\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4A8A27-D52C-4CBC-A518-D296FA51F709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EACB04-52AE-4C04-9453-769A9281A334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Debug Questions" sheetId="1" r:id="rId1"/>
-    <sheet name="Example" sheetId="3" r:id="rId2"/>
+    <sheet name="Science Quiz" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="66">
   <si>
     <t>Question</t>
   </si>
@@ -230,13 +230,10 @@
     <t>True or False?</t>
   </si>
   <si>
-    <t>https://cdn.pixabay.com/photo/2019/05/18/13/34/twigs-4211837__480.jpg</t>
-  </si>
-  <si>
-    <t>Background_Image</t>
-  </si>
-  <si>
-    <t>Hint_Image</t>
+    <t>Hint Image</t>
+  </si>
+  <si>
+    <t>Background Image</t>
   </si>
 </sst>
 </file>
@@ -662,16 +659,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="64.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -697,7 +695,7 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I1" t="s">
         <v>65</v>
@@ -721,17 +719,11 @@
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(1, COUNTA(B2:E2))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <f t="shared" ref="G2:G13" ca="1" si="0">F2</f>
-        <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I2" t="s">
-        <v>64</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -752,11 +744,11 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F14" ca="1" si="1">RANDBETWEEN(1, COUNTA(B3:E3))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -777,11 +769,11 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -802,11 +794,11 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -827,11 +819,11 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -852,11 +844,11 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -877,11 +869,11 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -902,11 +894,11 @@
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -927,11 +919,11 @@
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -977,11 +969,11 @@
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1002,11 +994,11 @@
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1035,11 +1027,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F48D06-45C7-4F1D-A65F-A94638A50CA9}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1050,10 +1042,11 @@
     <col min="4" max="4" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="20" style="1"/>
+    <col min="7" max="7" width="64.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="20" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1075,8 +1068,14 @@
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -1099,7 +1098,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -1122,7 +1121,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
@@ -1145,7 +1144,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
@@ -1168,7 +1167,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1191,7 +1190,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>24</v>
       </c>
@@ -1214,7 +1213,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>25</v>
       </c>
@@ -1237,7 +1236,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
updated quiz creating documentation
</commit_message>
<xml_diff>
--- a/src/data/data.xlsx
+++ b/src/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\quiz-app\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1A4199-F32A-456E-B211-EF907AC08631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237827FA-A9A2-4785-8ECC-312A8470B076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4272" windowWidth="7968" windowHeight="7620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Debug Questions" sheetId="1" r:id="rId1"/>
@@ -655,7 +655,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,11 +713,11 @@
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(1, COUNTA(B2:E2))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <f t="shared" ref="G2:G7" ca="1" si="0">F2</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -739,11 +739,11 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F8" ca="1" si="1">RANDBETWEEN(1, COUNTA(B3:E3))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -764,11 +764,11 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -789,11 +789,11 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -839,11 +839,11 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -915,7 +915,7 @@
       </c>
       <c r="F11">
         <f t="shared" ref="F11" ca="1" si="3">RANDBETWEEN(1, COUNTA(B11:E11))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G11">
         <v>2</v>
@@ -936,7 +936,7 @@
       </c>
       <c r="F12">
         <f t="shared" ref="F12:F13" ca="1" si="4">RANDBETWEEN(1, COUNTA(B12:E12))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <v>3</v>
@@ -957,7 +957,7 @@
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G13">
         <v>4</v>

</xml_diff>

<commit_message>
Added all samsat quizzes
</commit_message>
<xml_diff>
--- a/src/data/data.xlsx
+++ b/src/data/data.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\quiz-app\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237827FA-A9A2-4785-8ECC-312A8470B076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135264EF-9F96-48EC-A3FC-42021FB436C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15072" yWindow="3852" windowWidth="7968" windowHeight="7620" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Debug Questions" sheetId="1" r:id="rId1"/>
-    <sheet name="Science Quiz" sheetId="3" r:id="rId2"/>
+    <sheet name="Cyber Security" sheetId="4" r:id="rId2"/>
+    <sheet name="Tesla Coils" sheetId="5" r:id="rId3"/>
+    <sheet name="Andy Robot" sheetId="6" r:id="rId4"/>
+    <sheet name="Advanced Manufacturing" sheetId="7" r:id="rId5"/>
+    <sheet name="Augmented Reality" sheetId="8" r:id="rId6"/>
+    <sheet name="Autonomous Vehicle" sheetId="9" r:id="rId7"/>
+    <sheet name="Critical Infrastructure" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="297">
   <si>
     <t>Question</t>
   </si>
@@ -228,6 +234,705 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>Cyber security affects (choose the best answer)</t>
+  </si>
+  <si>
+    <t>Just your email</t>
+  </si>
+  <si>
+    <t>Wi-fi</t>
+  </si>
+  <si>
+    <t>Anything offline</t>
+  </si>
+  <si>
+    <t>Anything using a computer. So like everything.</t>
+  </si>
+  <si>
+    <t>Even refrigerators have one these days.</t>
+  </si>
+  <si>
+    <t>Always click on links you receive in email, it could be urgent!</t>
+  </si>
+  <si>
+    <t>It depends</t>
+  </si>
+  <si>
+    <t>Yes, hurry!</t>
+  </si>
+  <si>
+    <t>DANGER!  NEVER!</t>
+  </si>
+  <si>
+    <t>What's email?</t>
+  </si>
+  <si>
+    <t>Caution with links is the best and only policy.</t>
+  </si>
+  <si>
+    <t>To work in cyber, you need</t>
+  </si>
+  <si>
+    <t>Some post-secondary education</t>
+  </si>
+  <si>
+    <t>A four-year degree</t>
+  </si>
+  <si>
+    <t>An advanced degree</t>
+  </si>
+  <si>
+    <t>Could be A, B, or C</t>
+  </si>
+  <si>
+    <t>There are many kinds of opportunities.</t>
+  </si>
+  <si>
+    <t>Cyber is only about devices, and never about physical systems.</t>
+  </si>
+  <si>
+    <t>Super FALSE!</t>
+  </si>
+  <si>
+    <t>Only for phones</t>
+  </si>
+  <si>
+    <t>Computers can make our real life better!</t>
+  </si>
+  <si>
+    <t>San Antonio has the ________ most certified information security professionals in the U.S.</t>
+  </si>
+  <si>
+    <t>2nd</t>
+  </si>
+  <si>
+    <t>5th</t>
+  </si>
+  <si>
+    <t>17th</t>
+  </si>
+  <si>
+    <t>Not a category</t>
+  </si>
+  <si>
+    <t>San Antonio is world class!</t>
+  </si>
+  <si>
+    <t>Some of the highest ranked cyber education programs in the world are in San Antonio.</t>
+  </si>
+  <si>
+    <t>YES!</t>
+  </si>
+  <si>
+    <t>San Antonio is Cyber City USA!</t>
+  </si>
+  <si>
+    <t>Who invented the Tesla Coil?</t>
+  </si>
+  <si>
+    <t>Alexander Graham Bell</t>
+  </si>
+  <si>
+    <t>Thomas Edison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tess Ocean from Los Angeles  </t>
+  </si>
+  <si>
+    <t>Nikola Tesla</t>
+  </si>
+  <si>
+    <t>Come on, you got this one!</t>
+  </si>
+  <si>
+    <t>What year was the Tesla Coil First Invented?</t>
+  </si>
+  <si>
+    <t>Demonstrated for the first time before Teddy Roosevelt was President.</t>
+  </si>
+  <si>
+    <t>What did Nikola Tesla study in college?</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>Poetry &amp; Literature</t>
+  </si>
+  <si>
+    <t>Biology</t>
+  </si>
+  <si>
+    <t>What field of study is closest to his research?</t>
+  </si>
+  <si>
+    <t>What causes SAMSAT's Tesla Coil's loud volume?</t>
+  </si>
+  <si>
+    <t>Electricity bolts exiting from the top</t>
+  </si>
+  <si>
+    <t>The Spark Gap</t>
+  </si>
+  <si>
+    <t>Surrounding air reacting to the electricity</t>
+  </si>
+  <si>
+    <t>Tesla Coils have no manners</t>
+  </si>
+  <si>
+    <t>Sound comes from sound waves in the _____.</t>
+  </si>
+  <si>
+    <t>Nikola Tesla's lifelong dream was wireless power transmission</t>
+  </si>
+  <si>
+    <t>That's impossible</t>
+  </si>
+  <si>
+    <t>A goal, but not a dream</t>
+  </si>
+  <si>
+    <t>True &amp; coming true.  Wireless phone charging!</t>
+  </si>
+  <si>
+    <t>Wireless is wi-fi only</t>
+  </si>
+  <si>
+    <t>He had a dream.</t>
+  </si>
+  <si>
+    <t>Nikola Tesla invented DC Power</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>Edison did.  Tesla invented AC power.</t>
+  </si>
+  <si>
+    <t>True, with Thomas Edison</t>
+  </si>
+  <si>
+    <t>No such thing as DC power</t>
+  </si>
+  <si>
+    <t>They argued over which was best.  Tesla's idea won.</t>
+  </si>
+  <si>
+    <t>This person is known as the Grandfather of Robotics for inventing the robot arm.</t>
+  </si>
+  <si>
+    <t>George Devol</t>
+  </si>
+  <si>
+    <t>Andy from Toy Story</t>
+  </si>
+  <si>
+    <t>The first commercial product was introduced in 1962.</t>
+  </si>
+  <si>
+    <t>The most common robot arm design has this many joints, not unlike a human arm.</t>
+  </si>
+  <si>
+    <t>Count how many joints you have from your shoulder to your index finger.</t>
+  </si>
+  <si>
+    <t>Robot arm applications include</t>
+  </si>
+  <si>
+    <t>Manufacturing</t>
+  </si>
+  <si>
+    <t>For learning and fun, like Andy Robot</t>
+  </si>
+  <si>
+    <t>Painting</t>
+  </si>
+  <si>
+    <t>All the above and more</t>
+  </si>
+  <si>
+    <t>Many, many uses for robot arms.</t>
+  </si>
+  <si>
+    <t>Robot Arms can get tired and need to take a break.</t>
+  </si>
+  <si>
+    <t>No.  They work and work and work.</t>
+  </si>
+  <si>
+    <t>False.  They need 8 hours sleep a night.</t>
+  </si>
+  <si>
+    <t>They need maintenance like any machine.</t>
+  </si>
+  <si>
+    <t>Let's ask the Robot Arm.</t>
+  </si>
+  <si>
+    <t>People get tired, machines need care.</t>
+  </si>
+  <si>
+    <t>The usual cost of a robot arm is</t>
+  </si>
+  <si>
+    <t>$2,500</t>
+  </si>
+  <si>
+    <t>$10,000</t>
+  </si>
+  <si>
+    <t>$5,000,000</t>
+  </si>
+  <si>
+    <t>$400,000</t>
+  </si>
+  <si>
+    <t>You could buy a house for this, or two…</t>
+  </si>
+  <si>
+    <t>There's a 72-foot tall robot at Tech Port San Antonio.</t>
+  </si>
+  <si>
+    <t>Yeah, right.  Please!</t>
+  </si>
+  <si>
+    <t>The CIA suspects alien origin.</t>
+  </si>
+  <si>
+    <t>It's at XYREC and paints airplanes.</t>
+  </si>
+  <si>
+    <t>It's name is Slim.</t>
+  </si>
+  <si>
+    <t>Tallest known robot in the world.</t>
+  </si>
+  <si>
+    <t>Advanced manufacturing is</t>
+  </si>
+  <si>
+    <t>anything using 3D printers</t>
+  </si>
+  <si>
+    <t>manufacturing using innovative technology</t>
+  </si>
+  <si>
+    <t>anything built after 2003</t>
+  </si>
+  <si>
+    <t>The building of computers</t>
+  </si>
+  <si>
+    <t>Innovate, innovate, innovate.</t>
+  </si>
+  <si>
+    <t>3D printing was first used in</t>
+  </si>
+  <si>
+    <t>The 2000's</t>
+  </si>
+  <si>
+    <t>The 1960's</t>
+  </si>
+  <si>
+    <t>The 1980's</t>
+  </si>
+  <si>
+    <t>It's been around awhile, but it was not Ben Franklin.</t>
+  </si>
+  <si>
+    <t>Another name for 3D printing is</t>
+  </si>
+  <si>
+    <t>Super 3D</t>
+  </si>
+  <si>
+    <t>Subtractive manufacturing</t>
+  </si>
+  <si>
+    <t>Additive manufacturing</t>
+  </si>
+  <si>
+    <t>360 Build</t>
+  </si>
+  <si>
+    <t>Layer by layer.</t>
+  </si>
+  <si>
+    <t>Inexpensive 3D printers usually make items using</t>
+  </si>
+  <si>
+    <t>Plastic</t>
+  </si>
+  <si>
+    <t>Rubber</t>
+  </si>
+  <si>
+    <t>Paper</t>
+  </si>
+  <si>
+    <t>Metal</t>
+  </si>
+  <si>
+    <t>It's one of manufacturing's most popular materials.</t>
+  </si>
+  <si>
+    <t>High-end 3D printers can use the following as source material</t>
+  </si>
+  <si>
+    <t>Metals</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>All of the above</t>
+  </si>
+  <si>
+    <t>If it can melt and go through a nozzle…</t>
+  </si>
+  <si>
+    <t>3D printouts are limited to 14.5 inches in any dimension</t>
+  </si>
+  <si>
+    <t>False, but bigger is rare</t>
+  </si>
+  <si>
+    <t>False-look close by for examples!</t>
+  </si>
+  <si>
+    <t>3D is measured in centimeters</t>
+  </si>
+  <si>
+    <t>They can take a while, but…</t>
+  </si>
+  <si>
+    <t>There's a thing called the Fourth Industrial Revolution</t>
+  </si>
+  <si>
+    <t>You made that up</t>
+  </si>
+  <si>
+    <t>We skipped the Third Industrial Revolution</t>
+  </si>
+  <si>
+    <t>It happens every July 4</t>
+  </si>
+  <si>
+    <t>Yes: connected devices and automation</t>
+  </si>
+  <si>
+    <t>Look it up…</t>
+  </si>
+  <si>
+    <t>Precision in manufacturing is best achieved with</t>
+  </si>
+  <si>
+    <t>Traditional measuring tools</t>
+  </si>
+  <si>
+    <t>Robots doing all the work</t>
+  </si>
+  <si>
+    <t>Laser technology</t>
+  </si>
+  <si>
+    <t>A protractor</t>
+  </si>
+  <si>
+    <t>These tools are extremely precise.</t>
+  </si>
+  <si>
+    <t>These can be made with 3D printing</t>
+  </si>
+  <si>
+    <t>Prosthetics</t>
+  </si>
+  <si>
+    <t>Human organ models</t>
+  </si>
+  <si>
+    <t>Tiny Houses</t>
+  </si>
+  <si>
+    <t>Yes, all the above</t>
+  </si>
+  <si>
+    <t>3D printers are amazing!</t>
+  </si>
+  <si>
+    <t>3D printers on the moon will make habitats from moon dirt</t>
+  </si>
+  <si>
+    <t>Good idea, but no</t>
+  </si>
+  <si>
+    <t>That's nuts</t>
+  </si>
+  <si>
+    <t>Yes, and SAMSAT has an exhibit</t>
+  </si>
+  <si>
+    <t>Only on Mars</t>
+  </si>
+  <si>
+    <t>Look around!</t>
+  </si>
+  <si>
+    <t>Boeing researcher Thomas Caudell coined this term</t>
+  </si>
+  <si>
+    <t>Sci-Fi Reality</t>
+  </si>
+  <si>
+    <t>Augmented Reality</t>
+  </si>
+  <si>
+    <t>Augmented Earth</t>
+  </si>
+  <si>
+    <t>Virtual Reality</t>
+  </si>
+  <si>
+    <t>What's the title of this quiz?</t>
+  </si>
+  <si>
+    <t>Ivan Sutherland created a head-mounted display in 1968 called</t>
+  </si>
+  <si>
+    <t>The Sword of Damocles</t>
+  </si>
+  <si>
+    <t>The AR Headset</t>
+  </si>
+  <si>
+    <t>Sutherland System</t>
+  </si>
+  <si>
+    <t>Virtual Fixtures</t>
+  </si>
+  <si>
+    <t>It was named after an ancient Greek story.</t>
+  </si>
+  <si>
+    <t>Augmented Reality has applications in</t>
+  </si>
+  <si>
+    <t>Architecture, urban design, education</t>
+  </si>
+  <si>
+    <t>Manufacturing, art, fitness, first response</t>
+  </si>
+  <si>
+    <t>Industrial design, maintenance</t>
+  </si>
+  <si>
+    <t>Yes!  All those</t>
+  </si>
+  <si>
+    <t>It's used in quite a few places.</t>
+  </si>
+  <si>
+    <t>Flight: Training, maintenance, design</t>
+  </si>
+  <si>
+    <t>Recreation: Games, tourism</t>
+  </si>
+  <si>
+    <t>Archaeology</t>
+  </si>
+  <si>
+    <t>I get it!  Can enhance any real world experience</t>
+  </si>
+  <si>
+    <t>This game you can play augments your real surroundings</t>
+  </si>
+  <si>
+    <t>Pokemon Go</t>
+  </si>
+  <si>
+    <t>Zelda</t>
+  </si>
+  <si>
+    <t>Match 3</t>
+  </si>
+  <si>
+    <t>Fortnight</t>
+  </si>
+  <si>
+    <t>There are outdoor scavenger tournaments</t>
+  </si>
+  <si>
+    <t>Five minutes from here, this company uses Augmented Reality during maintenance and repair operations</t>
+  </si>
+  <si>
+    <t>Plumbers with AR</t>
+  </si>
+  <si>
+    <t>SAMSAT</t>
+  </si>
+  <si>
+    <t>Maintenance &amp; Repair, Inc.</t>
+  </si>
+  <si>
+    <t>The Boeing Company</t>
+  </si>
+  <si>
+    <t>They employ thousands of San Antonio residents.</t>
+  </si>
+  <si>
+    <t>The term Critical Infrastructure refers to the essentials necessary for a society to function and ____.</t>
+  </si>
+  <si>
+    <t>be entertained</t>
+  </si>
+  <si>
+    <t>grow</t>
+  </si>
+  <si>
+    <t>go to Mars</t>
+  </si>
+  <si>
+    <t>take over the World</t>
+  </si>
+  <si>
+    <t>With a proper environment, what do plants do?</t>
+  </si>
+  <si>
+    <t>Which of the following is a Critical Infrastructure Sector?</t>
+  </si>
+  <si>
+    <t>Utilities</t>
+  </si>
+  <si>
+    <t>Public Safety</t>
+  </si>
+  <si>
+    <t>Space and Technology</t>
+  </si>
+  <si>
+    <t>All of the Above (and so much more!)</t>
+  </si>
+  <si>
+    <t>Other examples include transportation, healthcare, and national security.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Dams Sector is VERY important because it provides___ of the Northwest United States' electricity. </t>
+  </si>
+  <si>
+    <t>The Dams Sector also protects 43% of U.S.A's population from flooding.</t>
+  </si>
+  <si>
+    <t>The Education Subsector is found under which sector?</t>
+  </si>
+  <si>
+    <t>Government Facilities</t>
+  </si>
+  <si>
+    <t>The Smarty Pants Sector</t>
+  </si>
+  <si>
+    <t>Information Technology</t>
+  </si>
+  <si>
+    <t>Communications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This sector includes locations owned or leased by federal, state, local, and tribal governments. </t>
+  </si>
+  <si>
+    <t>Why is the Transportation Systems Sector important?</t>
+  </si>
+  <si>
+    <t>Trains go choo-choo</t>
+  </si>
+  <si>
+    <t>It ensures safe and fast travel</t>
+  </si>
+  <si>
+    <t>It repairs our cars and airplanes</t>
+  </si>
+  <si>
+    <t>It transports dangerous chemicals</t>
+  </si>
+  <si>
+    <t>This sector includes the Transit and Passenger Rail subsector.</t>
+  </si>
+  <si>
+    <t>Is the Nuclear Reactor, Materials, and Waste Sector only used to create electricity?</t>
+  </si>
+  <si>
+    <t>Yes!</t>
+  </si>
+  <si>
+    <t>Maybe? (Check out the hint)</t>
+  </si>
+  <si>
+    <t>That sector doesn't exist...</t>
+  </si>
+  <si>
+    <t>NO!!!</t>
+  </si>
+  <si>
+    <t>This sector also provides the medical isotopes for cancer treatment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Water and Wastewater sector provides drinkable water to more than ___ of the U.S population. </t>
+  </si>
+  <si>
+    <t>About 75% of the U.S.A's population depends on this sector for sewage treatment too!</t>
+  </si>
+  <si>
+    <t>The ____ Sector protects all sectors of the economy from hazards such as terrorism, infectious disease outbreaks, and natural disasters.</t>
+  </si>
+  <si>
+    <t>Healthcare and Public Health</t>
+  </si>
+  <si>
+    <t>Emergency Services</t>
+  </si>
+  <si>
+    <t>Commercial Facilities</t>
+  </si>
+  <si>
+    <t>Defense and National Security</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> This sector is dependent on EMERGENCY SERVICES (and other sectors too)</t>
+  </si>
+  <si>
+    <t>What kinds of things can pose a threat to Critical Infrastructure?</t>
+  </si>
+  <si>
+    <t>A. Natural Disasters</t>
+  </si>
+  <si>
+    <t>Scooby-Do Super Villains</t>
+  </si>
+  <si>
+    <t>B. Cyber Attacks</t>
+  </si>
+  <si>
+    <t>A and B</t>
+  </si>
+  <si>
+    <t>These threaten a variety of sectors such as energy, food, and transportation.</t>
+  </si>
+  <si>
+    <t>Overall, how many sectors of Critical Infrastructure do you think currently exist?</t>
+  </si>
+  <si>
+    <t>This number is divisible by 4!</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
@@ -237,7 +942,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,6 +960,19 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -322,60 +1040,109 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{1417BBD8-0BD2-4D3C-8292-0430C7786C3F}"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -653,9 +1420,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,11 +1480,11 @@
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(1, COUNTA(B2:E2))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <f t="shared" ref="G2:G7" ca="1" si="0">F2</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -764,11 +1531,11 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -814,11 +1581,11 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -839,21 +1606,21 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="C8" s="11" t="b">
+      <c r="B8" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F8">
@@ -868,15 +1635,15 @@
       <c r="A9" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="C9" s="11" t="b">
+      <c r="B9" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F9">
         <f t="shared" ref="F9:F10" ca="1" si="2">RANDBETWEEN(1, COUNTA(B9:E9))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -886,15 +1653,15 @@
       <c r="A10" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10" s="11" t="b">
+      <c r="B10" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <v>3</v>
@@ -904,10 +1671,10 @@
       <c r="A11" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="3" t="s">
         <v>62</v>
       </c>
       <c r="D11" t="s">
@@ -915,7 +1682,7 @@
       </c>
       <c r="F11">
         <f t="shared" ref="F11" ca="1" si="3">RANDBETWEEN(1, COUNTA(B11:E11))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>2</v>
@@ -925,10 +1692,10 @@
       <c r="A12" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="3" t="s">
         <v>62</v>
       </c>
       <c r="D12" t="s">
@@ -946,10 +1713,10 @@
       <c r="A13" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="3" t="s">
         <v>62</v>
       </c>
       <c r="D13" t="s">
@@ -970,252 +1737,1607 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F48D06-45C7-4F1D-A65F-A94638A50CA9}">
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0BA600E-274F-4667-9934-8713008D4981}">
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="76.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20" style="1"/>
-    <col min="2" max="2" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="76" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="64.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="20" style="1"/>
+    <col min="7" max="7" width="37.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="76.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1">
+      <c r="B1" s="5">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5">
         <v>2</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="5">
         <v>3</v>
       </c>
-      <c r="E1" s="1">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="5">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="19">
+        <v>4</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="12">
+        <v>3</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="12">
+        <v>4</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="13">
+        <v>3</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>296</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF9A9145-D223-47D0-9FDF-D2696EF67A84}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="52.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="59.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1891</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1901</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1851</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1923</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C05F4597-686E-4A80-AF3D-D7D6C0D4F953}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="68.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="2">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="2">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="41">
+        <v>3</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="F6" s="42">
+        <v>4</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="F7" s="43">
+        <v>3</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE430373-6139-4B49-8ACC-28A698F1E95A}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="F2" s="11">
+        <v>2</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1767</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3" s="13">
+        <v>4</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="F4" s="12">
+        <v>3</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="F5" s="12">
+        <v>1</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="F6" s="11">
+        <v>4</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="F7" s="11">
+        <v>3</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="F8" s="11">
+        <v>4</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="F9" s="11">
+        <v>3</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="F10" s="11">
+        <v>4</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="F11" s="11">
+        <v>3</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F32EA077-6665-4999-86CE-DBAA5341FC2C}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="87.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5">
+        <v>4</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="F2" s="13">
+        <v>2</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="F3" s="13">
+        <v>1</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="F4" s="39">
+        <v>4</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="F5" s="39">
+        <v>4</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="F6" s="40">
+        <v>1</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>243</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="F7" s="40">
+        <v>4</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>247</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{305D2BA7-F155-49BD-A6B1-92074010BC17}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="90.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="64.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="38">
         <v>3</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="17" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="13">
         <v>3</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="12" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="1">
-        <v>4</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="39">
+        <v>4</v>
+      </c>
+      <c r="G4" s="12" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="5" t="s">
+      <c r="F5" s="36">
+        <v>1</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="13">
         <v>2</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="12" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="23">
         <v>3</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="24" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="B8" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="10" t="s">
+      <c r="F8" s="23">
+        <v>1</v>
+      </c>
+      <c r="G8" s="24" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="9" t="s">
+      <c r="B9" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" s="10" t="s">
+      <c r="F9" s="23">
+        <v>1</v>
+      </c>
+      <c r="G9" s="24" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:G6">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"false"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"true"</formula>
-    </cfRule>
-  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77CD7BAF-7026-451E-AAD7-D6A3B6547F4C}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="113.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="79.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="F2" s="12">
+        <v>2</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="F3" s="12">
+        <v>4</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="B4" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="C4" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="F4" s="36">
+        <v>2</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="F5" s="37">
+        <v>1</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="F6" s="12">
+        <v>2</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="F7" s="12">
+        <v>4</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="B8" s="14">
+        <v>0.95</v>
+      </c>
+      <c r="C8" s="14">
+        <v>2</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="E8" s="14">
+        <v>0.99</v>
+      </c>
+      <c r="F8" s="36">
+        <v>3</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="F9" s="12">
+        <v>1</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>290</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="F10" s="37">
+        <v>4</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="B11" s="12">
+        <v>5</v>
+      </c>
+      <c r="C11" s="12">
+        <v>50</v>
+      </c>
+      <c r="D11" s="12">
+        <v>16</v>
+      </c>
+      <c r="E11" s="12">
+        <v>25</v>
+      </c>
+      <c r="F11" s="12">
+        <v>3</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>295</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added all images for samsat
</commit_message>
<xml_diff>
--- a/src/data/data.xlsx
+++ b/src/data/data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\quiz-app\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135264EF-9F96-48EC-A3FC-42021FB436C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB66C48-C051-4D09-9F83-41D1AFF068F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15072" yWindow="3852" windowWidth="7968" windowHeight="7620" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Debug Questions" sheetId="1" r:id="rId1"/>
+    <sheet name="Demo Questions" sheetId="1" r:id="rId1"/>
     <sheet name="Cyber Security" sheetId="4" r:id="rId2"/>
     <sheet name="Tesla Coils" sheetId="5" r:id="rId3"/>
     <sheet name="Andy Robot" sheetId="6" r:id="rId4"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="305">
   <si>
     <t>Question</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Hint</t>
   </si>
   <si>
-    <t>Who?</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -65,24 +62,6 @@
     <t>Maybe</t>
   </si>
   <si>
-    <t>Absolutely</t>
-  </si>
-  <si>
-    <t>What?</t>
-  </si>
-  <si>
-    <t>When?</t>
-  </si>
-  <si>
-    <t>Where?</t>
-  </si>
-  <si>
-    <t>Why?</t>
-  </si>
-  <si>
-    <t>How?</t>
-  </si>
-  <si>
     <t>In the 1500s, Leonardo da Vinci invented a cart that followed a set path.</t>
   </si>
   <si>
@@ -215,18 +194,12 @@
     <t>Can you predict every future possibility?</t>
   </si>
   <si>
-    <t>True or False?</t>
-  </si>
-  <si>
     <t>Hint Image</t>
   </si>
   <si>
     <t>Background Image</t>
   </si>
   <si>
-    <t>A, B, or C?</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -933,6 +906,57 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>bgCar.jpg</t>
+  </si>
+  <si>
+    <t>bgCyber.jpg</t>
+  </si>
+  <si>
+    <t>bgTesla.jpg</t>
+  </si>
+  <si>
+    <t>bgArm.jpg</t>
+  </si>
+  <si>
+    <t>bgManufacturing.jpg</t>
+  </si>
+  <si>
+    <t>bgVR.jpg</t>
+  </si>
+  <si>
+    <t>bgIndustry.jpg</t>
+  </si>
+  <si>
+    <t>pCliff.jpg</t>
+  </si>
+  <si>
+    <t>pDavid.jpg</t>
+  </si>
+  <si>
+    <t>pLady.jpg</t>
+  </si>
+  <si>
+    <t>pTeacher.jpg</t>
+  </si>
+  <si>
+    <t>pYLady.png</t>
+  </si>
+  <si>
+    <t>pGirl.png</t>
+  </si>
+  <si>
+    <t>4 Choices</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>3 Choices</t>
+  </si>
+  <si>
+    <t>2 Choices</t>
   </si>
 </sst>
 </file>
@@ -1044,7 +1068,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1137,6 +1161,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1420,9 +1446,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1:I1"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1456,27 +1482,27 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="I1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>301</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(1, COUNTA(B2:E2))</f>
@@ -1490,245 +1516,68 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>303</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F8" ca="1" si="1">RANDBETWEEN(1, COUNTA(B3:E3))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>304</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="G5">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="G6">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="G7">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <f t="shared" ref="F9:F10" ca="1" si="2">RANDBETWEEN(1, COUNTA(B9:E9))</f>
-        <v>2</v>
-      </c>
-      <c r="G9">
-        <v>2</v>
-      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>3</v>
-      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11">
-        <f t="shared" ref="F11" ca="1" si="3">RANDBETWEEN(1, COUNTA(B11:E11))</f>
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>2</v>
-      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12">
-        <f t="shared" ref="F12:F13" ca="1" si="4">RANDBETWEEN(1, COUNTA(B12:E12))</f>
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>3</v>
-      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F13">
-        <f t="shared" ca="1" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="G13">
-        <v>4</v>
-      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1738,10 +1587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0BA600E-274F-4667-9934-8713008D4981}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="76.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1781,172 +1630,223 @@
         <v>2</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F2" s="19">
         <v>4</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>69</v>
+        <v>60</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="I2" s="44" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F3" s="12">
         <v>3</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>75</v>
+        <v>66</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="I3" s="44" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F4" s="12">
         <v>4</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>81</v>
+        <v>72</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="I4" s="44" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="6" t="b">
         <v>1</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F5" s="13">
         <v>3</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>85</v>
+        <v>76</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="I5" s="44" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="F6" s="25" t="s">
+        <v>287</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="17" t="s">
         <v>296</v>
       </c>
-      <c r="G6" s="12" t="s">
-        <v>91</v>
+      <c r="I6" s="44" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F7" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" s="17" t="s">
         <v>296</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>91</v>
+      <c r="I7" s="44" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F8" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" s="17" t="s">
         <v>296</v>
       </c>
-      <c r="G8" s="12" t="s">
-        <v>91</v>
-      </c>
+      <c r="I8" s="44" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H9" s="17"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H10" s="17"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H11" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1957,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF9A9145-D223-47D0-9FDF-D2696EF67A84}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1997,38 +1897,44 @@
         <v>2</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="F2" s="1">
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="I2" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B3" s="1">
         <v>1891</v>
@@ -2046,99 +1952,129 @@
         <v>1</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>102</v>
+        <v>93</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F4" s="1">
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F5" s="1">
         <v>3</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>114</v>
+        <v>105</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F6" s="1">
         <v>3</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="F7" s="1">
         <v>2</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>126</v>
+        <v>117</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -2150,8 +2086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C05F4597-686E-4A80-AF3D-D7D6C0D4F953}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2190,38 +2126,44 @@
         <v>2</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F2" s="2">
         <v>2</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>130</v>
+        <v>121</v>
+      </c>
+      <c r="H2" s="45" t="s">
+        <v>298</v>
+      </c>
+      <c r="I2" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B3" s="2">
         <v>6</v>
@@ -2239,99 +2181,129 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>132</v>
+        <v>123</v>
+      </c>
+      <c r="H3" s="45" t="s">
+        <v>298</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="F4" s="2">
         <v>4</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>138</v>
+        <v>129</v>
+      </c>
+      <c r="H4" s="45" t="s">
+        <v>298</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F5" s="41">
         <v>3</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>144</v>
+        <v>135</v>
+      </c>
+      <c r="H5" s="45" t="s">
+        <v>298</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="F6" s="42">
         <v>4</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>150</v>
+        <v>141</v>
+      </c>
+      <c r="H6" s="45" t="s">
+        <v>298</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="F7" s="43">
         <v>3</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>156</v>
+        <v>147</v>
+      </c>
+      <c r="H7" s="45" t="s">
+        <v>298</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -2343,8 +2315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE430373-6139-4B49-8ACC-28A698F1E95A}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2357,7 +2329,7 @@
     <col min="6" max="6" width="7.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -2383,240 +2355,300 @@
         <v>2</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="F2" s="11">
         <v>2</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>162</v>
+        <v>153</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="I2" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D3" s="6">
         <v>1767</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="F3" s="13">
         <v>4</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>167</v>
+        <v>158</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="F4" s="12">
         <v>3</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>173</v>
+        <v>164</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="F5" s="12">
         <v>1</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>179</v>
+        <v>170</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="F6" s="11">
         <v>4</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>184</v>
+        <v>175</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="F7" s="11">
         <v>3</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>189</v>
+        <v>180</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="F8" s="11">
         <v>4</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>195</v>
+        <v>186</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="F9" s="11">
         <v>3</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>201</v>
+        <v>192</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="F10" s="11">
         <v>4</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>207</v>
+        <v>198</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="F11" s="11">
         <v>3</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>213</v>
+        <v>204</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -2628,8 +2660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F32EA077-6665-4999-86CE-DBAA5341FC2C}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2668,148 +2700,184 @@
         <v>2</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="F2" s="13">
         <v>2</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>219</v>
+        <v>210</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>300</v>
+      </c>
+      <c r="I2" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="F3" s="13">
         <v>1</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>225</v>
+        <v>216</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>300</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="F4" s="39">
         <v>4</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>231</v>
+        <v>222</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>300</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="E5" s="25" t="s">
         <v>226</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>233</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>234</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>235</v>
       </c>
       <c r="F5" s="39">
         <v>4</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>231</v>
+        <v>222</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>300</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="F6" s="40">
         <v>1</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>241</v>
+        <v>232</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>300</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="F7" s="40">
         <v>4</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>247</v>
+        <v>238</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>300</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -2819,10 +2887,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{305D2BA7-F155-49BD-A6B1-92074010BC17}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2861,196 +2929,245 @@
         <v>2</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F2" s="38">
         <v>3</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>49</v>
+        <v>42</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="I2" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F3" s="13">
         <v>3</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>50</v>
+        <v>43</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F4" s="39">
         <v>4</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>51</v>
+        <v>44</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F5" s="36">
         <v>1</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>52</v>
+        <v>45</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F6" s="13">
         <v>2</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>53</v>
+        <v>46</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F7" s="23">
         <v>3</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>54</v>
+        <v>47</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B8" s="22" t="b">
         <v>1</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F8" s="23">
         <v>1</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>55</v>
+        <v>48</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F9" s="23">
         <v>1</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>56</v>
-      </c>
-    </row>
+        <v>49</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="28" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3060,8 +3177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77CD7BAF-7026-451E-AAD7-D6A3B6547F4C}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3101,61 +3218,73 @@
         <v>2</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="F2" s="12">
         <v>2</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>253</v>
+        <v>244</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="I2" s="44" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="F3" s="12">
         <v>4</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>259</v>
+        <v>250</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="I3" s="44" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B4" s="14">
         <v>0.25</v>
@@ -3173,81 +3302,105 @@
         <v>2</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>261</v>
+        <v>252</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="I4" s="44" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="F5" s="37">
         <v>1</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>267</v>
+        <v>258</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="I5" s="44" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="F6" s="12">
         <v>2</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>273</v>
+        <v>264</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="I6" s="44" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="F7" s="12">
         <v>4</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>279</v>
+        <v>270</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="I7" s="44" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="B8" s="14">
         <v>0.95</v>
@@ -3265,58 +3418,76 @@
         <v>3</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>281</v>
+        <v>272</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="I8" s="44" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="F9" s="12">
         <v>1</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>287</v>
+        <v>278</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="I9" s="44" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="F10" s="37">
         <v>4</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>293</v>
+        <v>284</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="I10" s="44" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B11" s="12">
         <v>5</v>
@@ -3334,7 +3505,13 @@
         <v>3</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>295</v>
+        <v>286</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="I11" s="44" t="s">
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hole in one golfer/issue32 (#33)
* Analytic System
Fixes #32

* store to session.data

* more fixes

* added stuff

* readme

* docs

* lock

* 2.0.2-0
</commit_message>
<xml_diff>
--- a/src/data/data.xlsx
+++ b/src/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\quiz-app\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\vscode_git\quiz-app\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AAA8554-8BBC-405B-9C5D-8315AAAEA6D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDC223E-F070-4BAE-A96E-186B3304BFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demo Questions" sheetId="1" r:id="rId1"/>
@@ -1080,37 +1080,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1123,11 +1119,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1140,41 +1136,36 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1458,7 +1449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C22" sqref="C21:C22"/>
     </sheetView>
@@ -1518,13 +1509,12 @@
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(1, COUNTA(B2:E2))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <f t="shared" ref="G2:G4" ca="1" si="0">F2</f>
-        <v>1</v>
-      </c>
-      <c r="I2" s="1"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -1541,11 +1531,11 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F4" ca="1" si="1">RANDBETWEEN(1, COUNTA(B3:E3))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -1560,36 +1550,36 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1601,264 +1591,263 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0BA600E-274F-4667-9934-8713008D4981}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F6:F8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="76.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="76" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="76.109375" style="1"/>
+    <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5">
+      <c r="B1">
         <v>1</v>
       </c>
-      <c r="C1" s="5">
+      <c r="C1">
         <v>2</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D1">
         <v>3</v>
       </c>
-      <c r="E1" s="5">
+      <c r="E1">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="15">
         <v>4</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I2" s="44" t="s">
+      <c r="I2" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="9">
         <v>3</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I3" s="44" t="s">
+      <c r="I3" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="9">
         <v>4</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I4" s="44" t="s">
+      <c r="I4" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6" t="b">
+      <c r="C5" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="10">
         <v>3</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I5" s="44" t="s">
+      <c r="I5" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I6" s="44" t="s">
+      <c r="I6" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I7" s="44" t="s">
+      <c r="I7" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I8" s="44" t="s">
+      <c r="I8" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H9" s="17"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H10" s="17"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H11" s="17"/>
+      <c r="H11" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -1881,64 +1870,64 @@
     <col min="3" max="3" width="31.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="59.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5">
+      <c r="B1">
         <v>1</v>
       </c>
-      <c r="C1" s="5">
+      <c r="C1">
         <v>2</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D1">
         <v>3</v>
       </c>
-      <c r="E1" s="5">
+      <c r="E1">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>91</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>296</v>
       </c>
       <c r="I2" t="s">
@@ -1946,147 +1935,147 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>1891</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>1901</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>1851</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3">
         <v>1923</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
         <v>296</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>97</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>98</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" t="s">
         <v>99</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
         <v>296</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>103</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5">
         <v>3</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" t="s">
         <v>105</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" t="s">
         <v>296</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>110</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6">
         <v>3</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" t="s">
         <v>111</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" t="s">
         <v>296</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>112</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>114</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>115</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>116</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7">
         <v>2</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" t="s">
         <v>296</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" t="s">
         <v>289</v>
       </c>
     </row>
@@ -2110,64 +2099,64 @@
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="61.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5">
+      <c r="B1">
         <v>1</v>
       </c>
-      <c r="C1" s="5">
+      <c r="C1">
         <v>2</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D1">
         <v>3</v>
       </c>
-      <c r="E1" s="5">
+      <c r="E1">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>2</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H2" s="45" t="s">
+      <c r="H2" s="38" t="s">
         <v>297</v>
       </c>
       <c r="I2" t="s">
@@ -2175,147 +2164,147 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>6</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>10</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>7</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>20</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="H3" s="38" t="s">
         <v>297</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>4</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="38" t="s">
         <v>297</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="F5" s="41">
+      <c r="F5" s="35">
         <v>3</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="H5" s="45" t="s">
+      <c r="H5" s="38" t="s">
         <v>297</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="F6" s="42">
+      <c r="F6" s="36">
         <v>4</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="H6" s="45" t="s">
+      <c r="H6" s="38" t="s">
         <v>297</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="F7" s="43">
+      <c r="F7" s="37">
         <v>3</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="H7" s="45" t="s">
+      <c r="H7" s="38" t="s">
         <v>297</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" t="s">
         <v>290</v>
       </c>
     </row>
@@ -2339,64 +2328,64 @@
     <col min="3" max="3" width="36.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5">
+      <c r="B1">
         <v>1</v>
       </c>
-      <c r="C1" s="5">
+      <c r="C1">
         <v>2</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D1">
         <v>3</v>
       </c>
-      <c r="E1" s="5">
+      <c r="E1">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="7">
         <v>2</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="5" t="s">
         <v>298</v>
       </c>
       <c r="I2" t="s">
@@ -2404,263 +2393,263 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="4">
         <v>1767</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="10">
         <v>4</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="9">
         <v>3</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="9">
         <v>1</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="7">
         <v>4</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="7">
         <v>3</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="7">
         <v>4</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="7">
         <v>3</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="7">
         <v>4</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="7">
         <v>3</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" t="s">
         <v>291</v>
       </c>
     </row>
@@ -2684,64 +2673,64 @@
     <col min="3" max="3" width="34.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" style="30" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="41.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5">
+      <c r="B1">
         <v>1</v>
       </c>
-      <c r="C1" s="5">
+      <c r="C1">
         <v>2</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D1">
         <v>3</v>
       </c>
-      <c r="E1" s="5">
+      <c r="E1">
         <v>4</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="10">
         <v>2</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="13" t="s">
         <v>299</v>
       </c>
       <c r="I2" t="s">
@@ -2749,147 +2738,147 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="10">
         <v>1</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="21" t="s">
         <v>219</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="F4" s="39">
+      <c r="F4" s="33">
         <v>4</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="F5" s="39">
+      <c r="F5" s="33">
         <v>4</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="F6" s="40">
+      <c r="F6" s="34">
         <v>1</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="22" t="s">
         <v>234</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="22" t="s">
         <v>235</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="F7" s="40">
+      <c r="F7" s="34">
         <v>4</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" t="s">
         <v>292</v>
       </c>
     </row>
@@ -2913,64 +2902,64 @@
     <col min="3" max="3" width="23.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="64.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5">
+      <c r="B1">
         <v>1</v>
       </c>
-      <c r="C1" s="5">
+      <c r="C1">
         <v>2</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D1">
         <v>3</v>
       </c>
-      <c r="E1" s="5">
+      <c r="E1">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="38">
+      <c r="F2" s="32">
         <v>3</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="14" t="s">
         <v>294</v>
       </c>
       <c r="I2" t="s">
@@ -2978,205 +2967,205 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="10">
         <v>3</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="14" t="s">
         <v>294</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="39">
+      <c r="F4" s="33">
         <v>4</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="14" t="s">
         <v>294</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="36">
+      <c r="F5" s="10">
         <v>1</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="14" t="s">
         <v>294</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="10">
         <v>2</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="14" t="s">
         <v>294</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="19">
         <v>3</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="G7" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="14" t="s">
         <v>294</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="22" t="b">
+      <c r="B8" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="19">
         <v>1</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="14" t="s">
         <v>294</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="19">
         <v>1</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="G9" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="14" t="s">
         <v>294</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" t="s">
         <v>287</v>
       </c>
     </row>
@@ -3196,334 +3185,333 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="113.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="79.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="113.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="79.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5">
+      <c r="B1">
         <v>1</v>
       </c>
-      <c r="C1" s="5">
+      <c r="C1">
         <v>2</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D1">
         <v>3</v>
       </c>
-      <c r="E1" s="5">
+      <c r="E1">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="9">
         <v>2</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I2" s="44" t="s">
+      <c r="I2" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="9">
         <v>4</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I3" s="44" t="s">
+      <c r="I3" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="11">
         <v>0.25</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="11">
         <v>0.6</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="11">
         <v>0.9</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="11">
         <v>0.75</v>
       </c>
-      <c r="F4" s="36">
+      <c r="F4" s="10">
         <v>2</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I4" s="44" t="s">
+      <c r="I4" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="F5" s="37">
+      <c r="F5" s="9">
         <v>1</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I5" s="44" t="s">
+      <c r="I5" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="9">
         <v>2</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I6" s="44" t="s">
+      <c r="I6" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="9">
         <v>4</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I7" s="44" t="s">
+      <c r="I7" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="11">
         <v>0.95</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="11">
         <v>2</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="11">
         <v>0.8</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="11">
         <v>0.99</v>
       </c>
-      <c r="F8" s="36">
+      <c r="F8" s="10">
         <v>3</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I8" s="44" t="s">
+      <c r="I8" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="9">
         <v>1</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I9" s="44" t="s">
+      <c r="I9" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="12" t="s">
         <v>280</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="F10" s="37">
+      <c r="F10" s="9">
         <v>4</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I10" s="44" t="s">
+      <c r="I10" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="9">
         <v>5</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="9">
         <v>50</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="9">
         <v>16</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="9">
         <v>25</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="9">
         <v>3</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I11" s="44" t="s">
+      <c r="I11" t="s">
         <v>293</v>
       </c>
     </row>

</xml_diff>